<commit_message>
Update 12 Added Textbox to display patient text file with edit and save options also added a function to the "New" command in menu to open a new window of diagnose
</commit_message>
<xml_diff>
--- a/Doctor.xlsx
+++ b/Doctor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>sfaa56%$</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -354,36 +357,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2">
+        <v>320620321</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>